<commit_message>
Loooots of work here with formatting and analysing the data into tables and charts 📈
</commit_message>
<xml_diff>
--- a/test-tools/TEST RESULTS/results/detecting_coldstart_timeout/Coldstart_Timeout_Results.xlsx
+++ b/test-tools/TEST RESULTS/results/detecting_coldstart_timeout/Coldstart_Timeout_Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisconnor/Sites/HONOURS_PROJECT/test-tools/results/detecting_coldstart_timeout/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisconnor/Sites/HONOURS_PROJECT/test-tools/TEST RESULTS/results/detecting_coldstart_timeout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B91F0F-CA66-4A49-9295-751ADA474D50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07065F16-74CD-B14D-8128-C2AA5208A0F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{7B228886-DC3A-DB4A-9EB7-C1B3C5EFA577}"/>
+    <workbookView xWindow="51200" yWindow="4500" windowWidth="38400" windowHeight="21140" xr2:uid="{7B228886-DC3A-DB4A-9EB7-C1B3C5EFA577}"/>
   </bookViews>
   <sheets>
     <sheet name="JAVA" sheetId="2" r:id="rId1"/>
@@ -18,22 +18,12 @@
     <sheet name="PYTHON" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">JAVA!$F$2:$F$12</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">JAVA!$I$2:$I$12</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">NODE!$F$2:$F$12</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">PYTHON!$F$2:$F$12</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">JAVA!$F$2:$F$12</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">JAVA!$I$2:$I$12</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">NODE!$F$2:$F$12</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">PYTHON!$F$2:$F$12</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">JAVA!$F$2:$F$12</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">JAVA!$I$2:$I$12</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">JAVA!$F$2:$F$12</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">JAVA!$I$2:$I$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">JAVA!$A$1:$H$34</definedName>
     <definedName name="coldstart_timeout_results_java_POST_24_03_2019_1608" localSheetId="0">JAVA!$A$1:$I$12</definedName>
+    <definedName name="coldstart_timeout_results_node_POST_24_03_2019_1607" localSheetId="0">JAVA!$A$13:$H$23</definedName>
     <definedName name="coldstart_timeout_results_node_POST_24_03_2019_1607" localSheetId="1">NODE!$A$2:$H$12</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{2227448B-F4CE-124B-9520-B28C5DC0F6D6}" name="coldstart_timeout_results_java_POST_24-03-2019_1608" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/chrisconnor/Sites/HONOURS_PROJECT/test-tools/results/detecting_coldstart_timeout/coldstart_timeout_results_java_POST_24-03-2019_1608.txt">
+    <textPr sourceFile="/Users/chrisconnor/Sites/HONOURS_PROJECT/test-tools/results/detecting_coldstart_timeout/coldstart_timeout_results_java_POST_24-03-2019_1608.txt">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -66,7 +56,19 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{535B64AC-3442-F04B-B6BF-3E9F3853CD47}" name="coldstart_timeout_results_node_POST_24-03-2019_1607" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/chrisconnor/Sites/HONOURS_PROJECT/test-tools/results/detecting_coldstart_timeout/coldstart_timeout_results_node_POST_24-03-2019_1607.txt">
+    <textPr sourceFile="/Users/chrisconnor/Sites/HONOURS_PROJECT/test-tools/results/detecting_coldstart_timeout/coldstart_timeout_results_node_POST_24-03-2019_1607.txt">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" xr16:uid="{983AB4A8-02D3-F046-A20C-82F3FB7B45EF}" name="coldstart_timeout_results_node_POST_24-03-2019_16071" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/chrisconnor/Sites/HONOURS_PROJECT/test-tools/results/detecting_coldstart_timeout/coldstart_timeout_results_node_POST_24-03-2019_1607.txt">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -81,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="57">
   <si>
     <t>Time Interval</t>
   </si>
@@ -228,13 +230,37 @@
   </si>
   <si>
     <t>$(date)</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>MEDIAN</t>
+  </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>99p</t>
+  </si>
+  <si>
+    <t>Java</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -297,6 +323,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2880" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Cold</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> start timeout test</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -310,7 +366,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2880" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2880" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -362,6 +418,47 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>JAVA!$J$2:$J$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0 mins</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5 mins</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10 mins</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15 mins</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20 mins</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25 mins</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30 mins</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35 mins</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40 mins</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45 mins</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50 mins</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>JAVA!$F$2:$F$12</c:f>
@@ -441,6 +538,47 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>JAVA!$J$2:$J$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0 mins</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5 mins</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10 mins</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15 mins</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20 mins</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25 mins</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30 mins</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35 mins</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40 mins</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45 mins</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50 mins</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>NODE!$F$2:$F$12</c:f>
@@ -520,6 +658,47 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>JAVA!$J$2:$J$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0 mins</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5 mins</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10 mins</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15 mins</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20 mins</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25 mins</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30 mins</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35 mins</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40 mins</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45 mins</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50 mins</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>PYTHON!$F$2:$F$12</c:f>
@@ -589,6 +768,75 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" i="1"/>
+                  <a:t>Timeout Interval</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" i="1" baseline="0"/>
+                  <a:t> (minutes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2000" i="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.41374584006014792"/>
+              <c:y val="0.95130543628760433"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -610,7 +858,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -653,6 +901,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" i="1"/>
+                  <a:t>Duration (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -669,7 +972,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -697,7 +1000,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1331,16 +1634,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4343400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1369,10 +1672,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="coldstart_timeout_results_node_POST_24-03-2019_1607" connectionId="3" xr16:uid="{B67B9300-358C-9E45-A93E-89525FD51391}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="coldstart_timeout_results_java_POST_24-03-2019_1608" connectionId="1" xr16:uid="{14885A63-CDA6-6147-A8A7-9BB14BF47137}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="coldstart_timeout_results_node_POST_24-03-2019_1607" connectionId="2" xr16:uid="{FC6C2F07-14C4-8F4B-BB10-F19453C49E66}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -1673,13 +1980,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4504157-90B5-3F49-9C24-763D1729502A}">
-  <dimension ref="A1:I12"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="65.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
@@ -1692,7 +2000,7 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1721,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1749,8 +2057,12 @@
       <c r="I2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="str">
+        <f>CONCATENATE(I2," mins")</f>
+        <v>0 mins</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1778,8 +2090,12 @@
       <c r="I3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J12" si="0">CONCATENATE(I3," mins")</f>
+        <v>5 mins</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1807,8 +2123,12 @@
       <c r="I4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>10 mins</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1836,8 +2156,12 @@
       <c r="I5">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>15 mins</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1865,8 +2189,21 @@
       <c r="I6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>20 mins</v>
+      </c>
+      <c r="M6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1894,8 +2231,27 @@
       <c r="I7">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>25 mins</v>
+      </c>
+      <c r="L7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7">
+        <f>AVERAGE(IF($B:$B=$M$6,$F:$F))</f>
+        <v>1.4572244242424246</v>
+      </c>
+      <c r="N7">
+        <f t="array" ref="N7">AVERAGE(IF($B:$B=N$6,$F:$F))</f>
+        <v>0.70947572727272723</v>
+      </c>
+      <c r="O7">
+        <f t="array" ref="O7">AVERAGE(IF($B:$B=O$6,$F:$F))</f>
+        <v>0.73427909090909094</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1923,8 +2279,27 @@
       <c r="I8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>30 mins</v>
+      </c>
+      <c r="L8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8">
+        <f>MEDIAN(IF($B:$B=$M$6,$F:$F))</f>
+        <v>0.90278700000000001</v>
+      </c>
+      <c r="N8">
+        <f t="array" ref="N8">MEDIAN(IF($B:$B=N$6,$F:$F))</f>
+        <v>0.87962399999999996</v>
+      </c>
+      <c r="O8">
+        <f t="array" ref="O8">MEDIAN(IF($B:$B=O$6,$F:$F))</f>
+        <v>0.90278700000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1952,8 +2327,27 @@
       <c r="I9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>35 mins</v>
+      </c>
+      <c r="L9" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9">
+        <f t="array" ref="M9">MIN(IF($B:$B=$M$6,$F:$F))</f>
+        <v>0.27685300000000002</v>
+      </c>
+      <c r="N9">
+        <f t="array" ref="N9">MIN(IF($B:$B=N$6,$F:$F))</f>
+        <v>0.20096600000000001</v>
+      </c>
+      <c r="O9">
+        <f t="array" ref="O9">MIN(IF($B:$B=O$6,$F:$F))</f>
+        <v>0.229238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1981,8 +2375,27 @@
       <c r="I10">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>40 mins</v>
+      </c>
+      <c r="L10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10">
+        <f t="array" ref="M10">MAX(IF($B:$B=$M$6,$F:$F))</f>
+        <v>5.713991</v>
+      </c>
+      <c r="N10">
+        <f t="array" ref="N10">MAX(IF($B:$B=N$6,$F:$F))</f>
+        <v>1.608063</v>
+      </c>
+      <c r="O10">
+        <f t="array" ref="O10">MAX(IF($B:$B=O$6,$F:$F))</f>
+        <v>1.5815600000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2010,8 +2423,27 @@
       <c r="I11">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>45 mins</v>
+      </c>
+      <c r="L11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" t="b">
+        <f t="array" ref="M11">IF($B:$B=$M$6,$F:$F)</f>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f t="array" ref="N11">MAX(IF($B:$B=N$6,$F:$F))</f>
+        <v>1.608063</v>
+      </c>
+      <c r="O11">
+        <f t="array" ref="O11">MAX(IF($B:$B=O$6,$F:$F))</f>
+        <v>1.5815600000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2039,8 +2471,595 @@
       <c r="I12">
         <v>50</v>
       </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>50 mins</v>
+      </c>
+      <c r="M12" t="e">
+        <f>PERCENTILE(M11,0.99)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>200</v>
+      </c>
+      <c r="D13">
+        <v>0.149506</v>
+      </c>
+      <c r="E13">
+        <v>0.14951600000000001</v>
+      </c>
+      <c r="F13">
+        <v>0.87962399999999996</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>200</v>
+      </c>
+      <c r="D14">
+        <v>0.10914699999999999</v>
+      </c>
+      <c r="E14">
+        <v>0.10915800000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.20096600000000001</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
+      </c>
+      <c r="D15">
+        <v>0.146874</v>
+      </c>
+      <c r="E15">
+        <v>0.14690400000000001</v>
+      </c>
+      <c r="F15">
+        <v>0.25073899999999999</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>200</v>
+      </c>
+      <c r="D16">
+        <v>0.14591899999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.14593</v>
+      </c>
+      <c r="F16">
+        <v>0.257683</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>200</v>
+      </c>
+      <c r="D17">
+        <v>0.14247399999999999</v>
+      </c>
+      <c r="E17">
+        <v>0.14250099999999999</v>
+      </c>
+      <c r="F17">
+        <v>0.25255</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>200</v>
+      </c>
+      <c r="D18">
+        <v>0.40278399999999998</v>
+      </c>
+      <c r="E18">
+        <v>0.40279599999999999</v>
+      </c>
+      <c r="F18">
+        <v>0.58706800000000003</v>
+      </c>
+      <c r="G18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>200</v>
+      </c>
+      <c r="D19">
+        <v>0.15665599999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.15668299999999999</v>
+      </c>
+      <c r="F19">
+        <v>0.99895</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>200</v>
+      </c>
+      <c r="D20">
+        <v>0.15203900000000001</v>
+      </c>
+      <c r="E20">
+        <v>0.15204999999999999</v>
+      </c>
+      <c r="F20">
+        <v>0.93357699999999999</v>
+      </c>
+      <c r="G20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>200</v>
+      </c>
+      <c r="D21">
+        <v>0.15046100000000001</v>
+      </c>
+      <c r="E21">
+        <v>0.15047199999999999</v>
+      </c>
+      <c r="F21">
+        <v>1.608063</v>
+      </c>
+      <c r="G21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>200</v>
+      </c>
+      <c r="D22">
+        <v>0.156801</v>
+      </c>
+      <c r="E22">
+        <v>0.156836</v>
+      </c>
+      <c r="F22">
+        <v>0.91756400000000005</v>
+      </c>
+      <c r="G22" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>200</v>
+      </c>
+      <c r="D23">
+        <v>0.14585699999999999</v>
+      </c>
+      <c r="E23">
+        <v>0.14588699999999999</v>
+      </c>
+      <c r="F23">
+        <v>0.91744899999999996</v>
+      </c>
+      <c r="G23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24">
+        <v>200</v>
+      </c>
+      <c r="D24">
+        <v>0.118354</v>
+      </c>
+      <c r="E24">
+        <v>0.118364</v>
+      </c>
+      <c r="F24">
+        <v>0.96058200000000005</v>
+      </c>
+      <c r="G24" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <v>200</v>
+      </c>
+      <c r="D25">
+        <v>0.107712</v>
+      </c>
+      <c r="E25">
+        <v>0.107723</v>
+      </c>
+      <c r="F25">
+        <v>0.23600099999999999</v>
+      </c>
+      <c r="G25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26">
+        <v>200</v>
+      </c>
+      <c r="D26">
+        <v>0.13073100000000001</v>
+      </c>
+      <c r="E26">
+        <v>0.13075800000000001</v>
+      </c>
+      <c r="F26">
+        <v>0.26276300000000002</v>
+      </c>
+      <c r="G26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>200</v>
+      </c>
+      <c r="D27">
+        <v>0.145588</v>
+      </c>
+      <c r="E27">
+        <v>0.14559900000000001</v>
+      </c>
+      <c r="F27">
+        <v>0.26100299999999999</v>
+      </c>
+      <c r="G27" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>200</v>
+      </c>
+      <c r="D28">
+        <v>0.117217</v>
+      </c>
+      <c r="E28">
+        <v>0.117244</v>
+      </c>
+      <c r="F28">
+        <v>0.229238</v>
+      </c>
+      <c r="G28" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29">
+        <v>200</v>
+      </c>
+      <c r="D29">
+        <v>0.15615499999999999</v>
+      </c>
+      <c r="E29">
+        <v>0.15618199999999999</v>
+      </c>
+      <c r="F29">
+        <v>0.285495</v>
+      </c>
+      <c r="G29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>200</v>
+      </c>
+      <c r="D30">
+        <v>0.15517900000000001</v>
+      </c>
+      <c r="E30">
+        <v>0.15518899999999999</v>
+      </c>
+      <c r="F30">
+        <v>0.981352</v>
+      </c>
+      <c r="G30" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <v>200</v>
+      </c>
+      <c r="D31">
+        <v>0.15340500000000001</v>
+      </c>
+      <c r="E31">
+        <v>0.153416</v>
+      </c>
+      <c r="F31">
+        <v>0.90278700000000001</v>
+      </c>
+      <c r="G31" t="s">
+        <v>3</v>
+      </c>
+      <c r="H31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>200</v>
+      </c>
+      <c r="D32">
+        <v>0.14513100000000001</v>
+      </c>
+      <c r="E32">
+        <v>0.14514099999999999</v>
+      </c>
+      <c r="F32">
+        <v>1.5815600000000001</v>
+      </c>
+      <c r="G32" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33">
+        <v>200</v>
+      </c>
+      <c r="D33">
+        <v>0.15454499999999999</v>
+      </c>
+      <c r="E33">
+        <v>0.154557</v>
+      </c>
+      <c r="F33">
+        <v>1.0964400000000001</v>
+      </c>
+      <c r="G33" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34">
+        <v>200</v>
+      </c>
+      <c r="D34">
+        <v>0.14480599999999999</v>
+      </c>
+      <c r="E34">
+        <v>0.14483499999999999</v>
+      </c>
+      <c r="F34">
+        <v>1.279849</v>
+      </c>
+      <c r="G34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H34" xr:uid="{93FDCCE7-AB7E-EA4E-B056-23F44E4885D5}">
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="greaterThan" val="0"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -2052,10 +3071,10 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2:H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="67.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -2065,7 +3084,7 @@
     <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -2091,7 +3110,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2117,7 +3136,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2143,7 +3162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2169,7 +3188,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2195,7 +3214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2221,7 +3240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2247,7 +3266,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2273,7 +3292,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2299,7 +3318,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2325,7 +3344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2351,7 +3370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2387,10 +3406,10 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="63.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
@@ -2402,7 +3421,7 @@
     <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -2428,7 +3447,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -2454,7 +3473,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2480,7 +3499,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2506,7 +3525,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -2532,7 +3551,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -2558,7 +3577,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2584,7 +3603,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -2610,7 +3629,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2636,7 +3655,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2662,7 +3681,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2688,7 +3707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>28</v>
       </c>

</xml_diff>